<commit_message>
PV- 03/13/2023 - All GST changes done -Running code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham Bhumkar\Desktop\KWE_GST_Process\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\605245\Documents\UiPath\FBSG_RPA_TEL_AP_KWE_GST\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9903E35A-A29D-4B31-AD0F-4EA87546EEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9D4317-8E8E-4F27-B2B1-68688D59A584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="312">
   <si>
     <t>Name</t>
   </si>
@@ -286,9 +286,6 @@
     <t>SenderMailId2</t>
   </si>
   <si>
-    <t>shubham.bhumkar@innowise.us</t>
-  </si>
-  <si>
     <t>ZipFileExtension</t>
   </si>
   <si>
@@ -349,12 +346,6 @@
     <t>Record is not present for column</t>
   </si>
   <si>
-    <t>Inbox\2023-KWE Freight INV</t>
-  </si>
-  <si>
-    <t>KWE//GST Billing Invoice Summary Report with scanned copies-</t>
-  </si>
-  <si>
     <t>DescriptionColumn</t>
   </si>
   <si>
@@ -484,9 +475,6 @@
     <t>InvoiceDateBlock</t>
   </si>
   <si>
-    <t>HWAB_NOBlock</t>
-  </si>
-  <si>
     <t>TotalAmountBlock</t>
   </si>
   <si>
@@ -503,9 +491,6 @@
   </si>
   <si>
     <t>Status Report.xlsx</t>
-  </si>
-  <si>
-    <t>InvoiceNoBlock,InvoiceDateBlock,HWAB_NOBlock,TotalAmountBlock</t>
   </si>
   <si>
     <t>AbbyFileSheetName</t>
@@ -644,9 +629,6 @@
     <t>StatusReportAllFailBody</t>
   </si>
   <si>
-    <t>saksham.bendkhale@innowise.us</t>
-  </si>
-  <si>
     <t>AbbyWorkflowDelay</t>
   </si>
   <si>
@@ -896,9 +878,6 @@
     <t>AbbyOutputFileName</t>
   </si>
   <si>
-    <t>GST_AbbyOutput_</t>
-  </si>
-  <si>
     <t>Abby Output File Name</t>
   </si>
   <si>
@@ -953,13 +932,73 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>C:\Users\Shubham Bhumkar\Desktop\KWE_GST_Process\Shared Folder</t>
-  </si>
-  <si>
-    <t>C:\Users\Shubham Bhumkar\Desktop\KWE_GST_Process\Shared Folder\Abby Output</t>
-  </si>
-  <si>
-    <t>C:\Users\Shubham Bhumkar\Desktop\KWE_GST_Process\Shared Folder\Hot Folder</t>
+    <t>norman.lim@tel.com</t>
+  </si>
+  <si>
+    <t>AbbyOutputPermitNoFile</t>
+  </si>
+  <si>
+    <t>GST_AbbyOutput</t>
+  </si>
+  <si>
+    <t>Data_PermitNo</t>
+  </si>
+  <si>
+    <t>PermitNotPresent</t>
+  </si>
+  <si>
+    <t>Permit No. Not Present</t>
+  </si>
+  <si>
+    <t>Permit no not available BRE message</t>
+  </si>
+  <si>
+    <t>ExcelDateRangeFrom</t>
+  </si>
+  <si>
+    <t>ExcelDateRangeTo</t>
+  </si>
+  <si>
+    <t>Date Range FROM for Excel file</t>
+  </si>
+  <si>
+    <t>Date Range TO for Excel file</t>
+  </si>
+  <si>
+    <t>Inbox</t>
+  </si>
+  <si>
+    <t>C:\Box\External\POOJA\GST_UiPath\Output</t>
+  </si>
+  <si>
+    <t>C:\Users\605245\Documents\Abbyy\Hotfolders\GST</t>
+  </si>
+  <si>
+    <t>C:\Users\605245\Documents\Abbyy\Exports\GST\RPAFolder</t>
+  </si>
+  <si>
+    <t>KWE// GST Billing Invoice Summary Report with scanned copies</t>
+  </si>
+  <si>
+    <t>AbbyyOutputCheck</t>
+  </si>
+  <si>
+    <t>GST_AbbyyCheckFlag</t>
+  </si>
+  <si>
+    <t>HAWBNoBlock</t>
+  </si>
+  <si>
+    <t>InvoiceNoBlock,InvoiceDateBlock,HAWBNoBlock,TotalAmountBlock,BatchName,DocumentDate,DocumentName</t>
+  </si>
+  <si>
+    <t>SetAssetValue</t>
+  </si>
+  <si>
+    <t>Set Abbyy Asset value in Orchestrator</t>
+  </si>
+  <si>
+    <t>DelayForOutlook</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1029,6 +1068,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,16 +1385,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="56.109375" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="56.08984375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1402,7 +1442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1412,7 +1452,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1429,7 +1469,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>300</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>46</v>
@@ -1440,7 +1480,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>104</v>
+        <v>304</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
@@ -1451,10 +1491,10 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1462,10 +1502,10 @@
         <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>289</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1474,10 +1514,10 @@
         <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -1485,32 +1525,32 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1521,7 +1561,7 @@
         <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1533,7 +1573,7 @@
         <v>74</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -1544,479 +1584,518 @@
         <v>76</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
         <v>98</v>
       </c>
-      <c r="B28" t="s">
-        <v>99</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>308</v>
       </c>
       <c r="C34" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C38" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C39" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C50" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>307</v>
       </c>
       <c r="C51" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
         <v>150</v>
       </c>
-      <c r="B56" t="s">
-        <v>154</v>
-      </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C61" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C62" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C63" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C64" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>289</v>
       </c>
       <c r="C66" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C68" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B70" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C70" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B72" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C72" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" t="s">
+        <v>292</v>
+      </c>
+    </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B74" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B75" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="78" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
+        <v>296</v>
+      </c>
+      <c r="B77">
+        <v>13</v>
+      </c>
+      <c r="C77" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A78" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>299</v>
+      </c>
+    </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
+        <v>309</v>
+      </c>
+      <c r="B80" t="s">
+        <v>306</v>
+      </c>
+      <c r="C80" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B81" s="6"/>
+    </row>
+    <row r="82" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="83" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="84" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="85" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="86" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="87" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="88" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="89" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="90" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="91" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="92" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="93" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="94" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="95" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="96" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="97" ht="14.25" customHeight="1"/>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
@@ -2935,16 +3014,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2981,7 +3060,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2992,7 +3071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3185,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -3127,7 +3206,7 @@
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -3138,7 +3217,7 @@
         <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -3149,7 +3228,7 @@
         <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -3160,7 +3239,7 @@
         <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -3171,7 +3250,7 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -3182,7 +3261,7 @@
         <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -3193,7 +3272,7 @@
         <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -3204,7 +3283,7 @@
         <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -3215,219 +3294,229 @@
         <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
       <c r="C29" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="B30" t="s">
-        <v>88</v>
-      </c>
       <c r="C30" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C31" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
         <v>101</v>
       </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
       <c r="C32" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C40" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C41" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C42" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C44" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>293</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C48" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
         <v>64</v>
@@ -3436,7 +3525,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
@@ -3447,7 +3536,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
@@ -3458,7 +3547,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3470,7 +3559,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
@@ -3481,115 +3570,122 @@
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B56">
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C61" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C65" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C66" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B68">
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
+        <v>311</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+    </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4540,14 +4636,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4586,7 +4684,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>